<commit_message>
Se suben avances mantenedor usuario activo
</commit_message>
<xml_diff>
--- a/WebApplication1/ExcelFolder/EXCEL_CONDUCTOR_EN_RED.xlsx
+++ b/WebApplication1/ExcelFolder/EXCEL_CONDUCTOR_EN_RED.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CC1136-BAC6-4D64-B796-C3F33A4AC52A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6525E9-3157-4100-9C4B-EDFBD554C6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CB6288AE-06AE-465F-8E9E-6F28D11CD07E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CB6288AE-06AE-465F-8E9E-6F28D11CD07E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -69,13 +69,13 @@
     <t>DOS</t>
   </si>
   <si>
-    <t>16808962-7</t>
-  </si>
-  <si>
-    <t>ROBERTO</t>
-  </si>
-  <si>
-    <t>CORDOVA</t>
+    <t>17459567-4</t>
+  </si>
+  <si>
+    <t>SERGIO</t>
+  </si>
+  <si>
+    <t>SOTO</t>
   </si>
 </sst>
 </file>
@@ -439,7 +439,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:F13"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Se sube el envío de correo completo, notifica que se ha cargado el horario
</commit_message>
<xml_diff>
--- a/WebApplication1/ExcelFolder/EXCEL_CONDUCTOR_EN_RED.xlsx
+++ b/WebApplication1/ExcelFolder/EXCEL_CONDUCTOR_EN_RED.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandr\Desktop\Presentación Seminario 30-11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A69108-F69A-4B02-A789-D18977B99B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A3F981-FE26-404E-B527-6C265FBB3222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CB6288AE-06AE-465F-8E9E-6F28D11CD07E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="17">
   <si>
     <t>FECHA INICIO</t>
   </si>
@@ -72,7 +72,19 @@
     <t>Soto</t>
   </si>
   <si>
-    <t>DOS</t>
+    <t>UNO</t>
+  </si>
+  <si>
+    <t>16808962-7</t>
+  </si>
+  <si>
+    <t>Roberto</t>
+  </si>
+  <si>
+    <t>Cordova</t>
+  </si>
+  <si>
+    <t>LO ESPEJO</t>
   </si>
 </sst>
 </file>
@@ -433,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54286B2F-8F8B-4A1D-B837-ABCC2119E95E}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,7 +504,7 @@
         <v>12</v>
       </c>
       <c r="G2" s="1">
-        <v>44529</v>
+        <v>44536</v>
       </c>
       <c r="H2" s="2">
         <v>0.21180555555555555</v>
@@ -515,7 +527,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="1">
-        <v>44530</v>
+        <v>44537</v>
       </c>
       <c r="H3" s="2">
         <v>0.25347222222222199</v>
@@ -538,7 +550,7 @@
         <v>12</v>
       </c>
       <c r="G4" s="1">
-        <v>44531</v>
+        <v>44538</v>
       </c>
       <c r="H4" s="2">
         <v>0.29513888888888901</v>
@@ -561,7 +573,7 @@
         <v>12</v>
       </c>
       <c r="G5" s="1">
-        <v>44532</v>
+        <v>44539</v>
       </c>
       <c r="H5" s="2">
         <v>0.33680555555555602</v>
@@ -584,7 +596,7 @@
         <v>12</v>
       </c>
       <c r="G6" s="1">
-        <v>44533</v>
+        <v>44540</v>
       </c>
       <c r="H6" s="2">
         <v>0.37847222222222199</v>
@@ -607,7 +619,7 @@
         <v>12</v>
       </c>
       <c r="G7" s="1">
-        <v>44534</v>
+        <v>44541</v>
       </c>
       <c r="H7" s="2">
         <v>0.42013888888888901</v>
@@ -630,9 +642,170 @@
         <v>12</v>
       </c>
       <c r="G8" s="1">
-        <v>44535</v>
+        <v>44542</v>
       </c>
       <c r="H8" s="2">
+        <v>0.46180555555555602</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="1">
+        <v>44536</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.21180555555555555</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="1">
+        <v>44537</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.25347222222222199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="1">
+        <v>44538</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.29513888888888901</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="1">
+        <v>44539</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.33680555555555602</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="1">
+        <v>44540</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0.37847222222222199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="1">
+        <v>44541</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0.42013888888888901</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="1">
+        <v>44542</v>
+      </c>
+      <c r="H15" s="2">
         <v>0.46180555555555602</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se subeN CORRECCIONES EN DASHBOARD
</commit_message>
<xml_diff>
--- a/WebApplication1/ExcelFolder/EXCEL_CONDUCTOR_EN_RED.xlsx
+++ b/WebApplication1/ExcelFolder/EXCEL_CONDUCTOR_EN_RED.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandr\Desktop\Presentación Seminario 30-11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A3F981-FE26-404E-B527-6C265FBB3222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933E829E-FA6A-4177-BF52-82C926DA8B68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CB6288AE-06AE-465F-8E9E-6F28D11CD07E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="13">
   <si>
     <t>FECHA INICIO</t>
   </si>
@@ -48,9 +48,6 @@
     <t>NOMBRE TERMINAL INICIO</t>
   </si>
   <si>
-    <t>LO MARCOLETA</t>
-  </si>
-  <si>
     <t>APELLIDO PATERNO</t>
   </si>
   <si>
@@ -63,28 +60,19 @@
     <t>JORNADA</t>
   </si>
   <si>
-    <t>17459567-4</t>
-  </si>
-  <si>
-    <t>Sergio</t>
-  </si>
-  <si>
-    <t>Soto</t>
-  </si>
-  <si>
     <t>UNO</t>
   </si>
   <si>
+    <t xml:space="preserve">Roberto </t>
+  </si>
+  <si>
+    <t>Cordova</t>
+  </si>
+  <si>
     <t>16808962-7</t>
   </si>
   <si>
-    <t>Roberto</t>
-  </si>
-  <si>
-    <t>Cordova</t>
-  </si>
-  <si>
-    <t>LO ESPEJO</t>
+    <t>Lo Marcoleta</t>
   </si>
 </sst>
 </file>
@@ -445,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54286B2F-8F8B-4A1D-B837-ABCC2119E95E}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="I1" sqref="I1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,13 +451,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -478,7 +466,7 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -489,22 +477,22 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G2" s="1">
-        <v>44536</v>
+        <v>44543</v>
       </c>
       <c r="H2" s="2">
         <v>0.21180555555555555</v>
@@ -512,301 +500,140 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G3" s="1">
-        <v>44537</v>
+        <v>44544</v>
       </c>
       <c r="H3" s="2">
-        <v>0.25347222222222199</v>
+        <v>0.21527777777777779</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G4" s="1">
-        <v>44538</v>
+        <v>44545</v>
       </c>
       <c r="H4" s="2">
-        <v>0.29513888888888901</v>
+        <v>0.21875</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G5" s="1">
-        <v>44539</v>
+        <v>44546</v>
       </c>
       <c r="H5" s="2">
-        <v>0.33680555555555602</v>
+        <v>0.22222222222222199</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
       <c r="D6" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G6" s="1">
-        <v>44540</v>
+        <v>44547</v>
       </c>
       <c r="H6" s="2">
-        <v>0.37847222222222199</v>
+        <v>0.225694444444444</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
       <c r="D7" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G7" s="1">
-        <v>44541</v>
+        <v>44548</v>
       </c>
       <c r="H7" s="2">
-        <v>0.42013888888888901</v>
+        <v>0.22916666666666699</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
       <c r="D8" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G8" s="1">
-        <v>44542</v>
+        <v>44549</v>
       </c>
       <c r="H8" s="2">
-        <v>0.46180555555555602</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="1">
-        <v>44536</v>
-      </c>
-      <c r="H9" s="2">
-        <v>0.21180555555555555</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="1">
-        <v>44537</v>
-      </c>
-      <c r="H10" s="2">
-        <v>0.25347222222222199</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="1">
-        <v>44538</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0.29513888888888901</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="1">
-        <v>44539</v>
-      </c>
-      <c r="H12" s="2">
-        <v>0.33680555555555602</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="1">
-        <v>44540</v>
-      </c>
-      <c r="H13" s="2">
-        <v>0.37847222222222199</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="1">
-        <v>44541</v>
-      </c>
-      <c r="H14" s="2">
-        <v>0.42013888888888901</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="1">
-        <v>44542</v>
-      </c>
-      <c r="H15" s="2">
-        <v>0.46180555555555602</v>
+        <v>0.23263888888888901</v>
       </c>
     </row>
   </sheetData>

</xml_diff>